<commit_message>
content read from file
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -20,9 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>mln02koushik@gmail.com</t>
+  </si>
+  <si>
+    <t>swapnanilsaha26@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -196,10 +199,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -212,11 +215,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1" display="mln02koushik@gmail.com"/>
+    <hyperlink ref="A2" r:id="rId2" display="swapnanilsaha26@gmail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>